<commit_message>
Updated original reference Excel files with necessary project id = 0 + annotated PRCdev column as extra input
</commit_message>
<xml_diff>
--- a/PMConverter/administration/1_Project data input sheet.xlsx
+++ b/PMConverter/administration/1_Project data input sheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38020" yWindow="-5600" windowWidth="29520" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="-38025" yWindow="-5595" windowWidth="29520" windowHeight="16440" tabRatio="500" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline Schedule" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="TP6" sheetId="9" r:id="rId9"/>
     <sheet name="TP7" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -888,11 +888,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1300,7 +1300,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="7" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1327,13 +1327,13 @@
     <xf numFmtId="22" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="7" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="7" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="7" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1402,97 +1402,97 @@
     </xf>
   </cellXfs>
   <cellStyles count="183">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1584,7 +1584,7 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1912,23 +1912,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.875" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1954,7 +1954,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="21">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1990,7 +1990,9 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
       <c r="B3" s="8" t="s">
         <v>268</v>
       </c>
@@ -2195,7 +2197,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="21">
       <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
@@ -2324,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" ht="21">
       <c r="A14" s="7" t="s">
         <v>54</v>
       </c>
@@ -2362,7 +2364,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="21">
       <c r="A15" s="7" t="s">
         <v>60</v>
       </c>
@@ -2397,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="21">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2449,7 +2451,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="21">
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
@@ -2484,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="21">
       <c r="A19" s="7" t="s">
         <v>76</v>
       </c>
@@ -2519,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="21">
       <c r="A20" s="7" t="s">
         <v>80</v>
       </c>
@@ -2554,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="21">
       <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
@@ -2606,7 +2608,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="21">
       <c r="A23" s="7" t="s">
         <v>91</v>
       </c>
@@ -2726,7 +2728,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="33">
+    <row r="27" spans="1:11" ht="31.5">
       <c r="A27" s="7" t="s">
         <v>106</v>
       </c>
@@ -2951,7 +2953,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" ht="55">
+    <row r="34" spans="1:11" ht="52.5">
       <c r="A34" s="7" t="s">
         <v>132</v>
       </c>
@@ -3569,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="22">
+    <row r="54" spans="1:11" ht="21">
       <c r="A54" s="7" t="s">
         <v>189</v>
       </c>
@@ -3600,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="22">
+    <row r="55" spans="1:11" ht="21">
       <c r="A55" s="7" t="s">
         <v>192</v>
       </c>
@@ -3845,21 +3847,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -3889,7 +3891,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3910,7 +3912,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>
@@ -5024,21 +5028,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5053,7 +5057,7 @@
       </c>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="21">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5328,18 +5332,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5354,7 +5358,7 @@
       <c r="E1" s="34"/>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="21">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5375,7 +5379,9 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
       <c r="B3" s="27" t="s">
         <v>269</v>
       </c>
@@ -6488,21 +6494,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -6532,7 +6538,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -6553,7 +6559,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>
@@ -7575,21 +7583,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -7619,7 +7627,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -7640,7 +7648,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>
@@ -8668,21 +8678,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -8712,7 +8722,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -8733,7 +8743,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>
@@ -9771,21 +9783,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -9815,7 +9827,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -9836,7 +9848,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>
@@ -10882,21 +10896,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -10926,7 +10940,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -10947,7 +10961,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>
@@ -11997,21 +12013,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -12041,7 +12057,7 @@
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="22" customHeight="1">
+    <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -12062,7 +12078,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
Update widths of reference Excel sheets
</commit_message>
<xml_diff>
--- a/PMConverter/administration/1_Project data input sheet.xlsx
+++ b/PMConverter/administration/1_Project data input sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38025" yWindow="-5595" windowWidth="29520" windowHeight="16440" tabRatio="500" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-38025" yWindow="-5595" windowWidth="29520" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline Schedule" sheetId="1" r:id="rId1"/>
@@ -1915,19 +1915,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="8" width="18.625" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.875" customWidth="1"/>
+    <col min="10" max="10" width="9.375" customWidth="1"/>
     <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3850,7 +3850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -3858,10 +3858,10 @@
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -5040,9 +5040,9 @@
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.625" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
+    <col min="6" max="6" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6505,10 +6505,10 @@
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -7594,10 +7594,10 @@
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -8689,10 +8689,10 @@
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -9794,10 +9794,10 @@
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -10900,17 +10900,17 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -12024,10 +12024,10 @@
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">

</xml_diff>